<commit_message>
Added error handling for faculty
</commit_message>
<xml_diff>
--- a/FeedbackDatabaseDesign.xlsx
+++ b/FeedbackDatabaseDesign.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\feedback\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Feedback\feedback\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" tabRatio="569"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7755" tabRatio="569"/>
   </bookViews>
   <sheets>
     <sheet name="ERDesign" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="129">
   <si>
     <t>effective_from</t>
   </si>
@@ -401,13 +401,19 @@
   </si>
   <si>
     <t>feedback_weighting</t>
+  </si>
+  <si>
+    <t>Redundant storage of start date and end date</t>
+  </si>
+  <si>
+    <t>This is the only primary key, what is its significance?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,8 +443,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,6 +474,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -576,7 +603,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -650,6 +677,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -746,23 +782,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -798,23 +817,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -993,22 +995,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="G170" sqref="G170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="80.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="80.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1023,7 +1025,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
@@ -1031,7 +1033,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -1051,7 +1053,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1072,7 +1074,7 @@
       </c>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1097,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="6"/>
@@ -1103,7 +1105,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="6"/>
@@ -1111,7 +1113,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="6"/>
@@ -1119,7 +1121,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1131,7 +1133,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
@@ -1139,7 +1141,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1159,7 +1161,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1180,7 +1182,7 @@
       </c>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -1203,7 +1205,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1226,7 +1228,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1238,7 +1240,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
@@ -1246,7 +1248,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
@@ -1266,7 +1268,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1289,7 +1291,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
@@ -1309,7 +1311,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -1329,7 +1331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
@@ -1349,7 +1351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
@@ -1369,7 +1371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
@@ -1389,7 +1391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1409,7 +1411,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
@@ -1429,7 +1431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
@@ -1441,7 +1443,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="2"/>
@@ -1449,7 +1451,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>15</v>
       </c>
@@ -1469,7 +1471,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -1492,7 +1494,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1517,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>48</v>
       </c>
@@ -1535,7 +1537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>13</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="3"/>
       <c r="C42" s="2"/>
@@ -1558,7 +1560,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>15</v>
       </c>
@@ -1578,7 +1580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
@@ -1599,7 +1601,7 @@
       </c>
       <c r="G44" s="16"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -1622,7 +1624,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>29</v>
       </c>
@@ -1645,7 +1647,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>45</v>
       </c>
@@ -1665,7 +1667,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>13</v>
       </c>
@@ -1680,7 +1682,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="3"/>
       <c r="C52" s="2"/>
@@ -1688,7 +1690,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="2"/>
     </row>
-    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>15</v>
       </c>
@@ -1708,7 +1710,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>6</v>
       </c>
@@ -1728,7 +1730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>52</v>
       </c>
@@ -1751,7 +1753,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>13</v>
       </c>
@@ -1763,7 +1765,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="2"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="3"/>
       <c r="C60" s="2"/>
@@ -1771,7 +1773,7 @@
       <c r="E60" s="3"/>
       <c r="F60" s="2"/>
     </row>
-    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>15</v>
       </c>
@@ -1791,7 +1793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>7</v>
       </c>
@@ -1814,7 +1816,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>54</v>
       </c>
@@ -1834,7 +1836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>13</v>
       </c>
@@ -1846,7 +1848,7 @@
       <c r="E67" s="3"/>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="3"/>
       <c r="C68" s="2"/>
@@ -1854,7 +1856,7 @@
       <c r="E68" s="3"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>15</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>40</v>
       </c>
@@ -1897,7 +1899,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>43</v>
       </c>
@@ -1920,7 +1922,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>5</v>
       </c>
@@ -1940,7 +1942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>46</v>
       </c>
@@ -1960,7 +1962,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>47</v>
       </c>
@@ -1980,7 +1982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>6</v>
       </c>
@@ -2003,7 +2005,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>7</v>
       </c>
@@ -2026,7 +2028,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>49</v>
       </c>
@@ -2049,7 +2051,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>50</v>
       </c>
@@ -2069,7 +2071,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>13</v>
       </c>
@@ -2081,7 +2083,7 @@
       <c r="E82" s="3"/>
       <c r="F82" s="2"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="3"/>
       <c r="C83" s="2"/>
@@ -2089,7 +2091,7 @@
       <c r="E83" s="3"/>
       <c r="F83" s="2"/>
     </row>
-    <row r="84" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>15</v>
       </c>
@@ -2109,7 +2111,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>40</v>
       </c>
@@ -2129,7 +2131,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>43</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>46</v>
       </c>
@@ -2169,7 +2171,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
         <v>55</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
         <v>63</v>
       </c>
@@ -2212,7 +2214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>56</v>
       </c>
@@ -2232,7 +2234,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>13</v>
       </c>
@@ -2244,7 +2246,7 @@
       <c r="E94" s="3"/>
       <c r="F94" s="2"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="3"/>
       <c r="C95" s="2"/>
@@ -2252,7 +2254,7 @@
       <c r="E95" s="3"/>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>15</v>
       </c>
@@ -2272,7 +2274,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>59</v>
       </c>
@@ -2292,7 +2294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
         <v>73</v>
       </c>
@@ -2312,7 +2314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="11"/>
       <c r="B99" s="12"/>
       <c r="C99" s="11"/>
@@ -2320,7 +2322,7 @@
       <c r="E99" s="12"/>
       <c r="F99" s="11"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="11"/>
       <c r="B100" s="12"/>
       <c r="C100" s="11"/>
@@ -2328,7 +2330,7 @@
       <c r="E100" s="12"/>
       <c r="F100" s="11"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="11"/>
       <c r="B101" s="12"/>
       <c r="C101" s="11"/>
@@ -2336,7 +2338,7 @@
       <c r="E101" s="12"/>
       <c r="F101" s="11"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>13</v>
       </c>
@@ -2348,7 +2350,7 @@
       <c r="E102" s="3"/>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="3"/>
       <c r="C103" s="2"/>
@@ -2356,7 +2358,7 @@
       <c r="E103" s="3"/>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>15</v>
       </c>
@@ -2376,7 +2378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
         <v>0</v>
       </c>
@@ -2396,7 +2398,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -2416,7 +2418,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>60</v>
       </c>
@@ -2436,7 +2438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>61</v>
       </c>
@@ -2456,7 +2458,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>13</v>
       </c>
@@ -2468,7 +2470,7 @@
       <c r="E112" s="3"/>
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="3"/>
       <c r="C113" s="2"/>
@@ -2476,7 +2478,7 @@
       <c r="E113" s="3"/>
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>15</v>
       </c>
@@ -2496,7 +2498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>10</v>
       </c>
@@ -2519,7 +2521,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>40</v>
       </c>
@@ -2539,7 +2541,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>43</v>
       </c>
@@ -2559,7 +2561,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>46</v>
       </c>
@@ -2579,7 +2581,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>2</v>
       </c>
@@ -2599,7 +2601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>5</v>
       </c>
@@ -2619,7 +2621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>64</v>
       </c>
@@ -2642,7 +2644,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>30</v>
       </c>
@@ -2662,7 +2664,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>13</v>
       </c>
@@ -2674,7 +2676,7 @@
       <c r="E126" s="3"/>
       <c r="F126" s="2"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="3"/>
       <c r="C127" s="2"/>
@@ -2682,7 +2684,7 @@
       <c r="E127" s="3"/>
       <c r="F127" s="2"/>
     </row>
-    <row r="128" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>15</v>
       </c>
@@ -2702,7 +2704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>66</v>
       </c>
@@ -2722,7 +2724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>67</v>
       </c>
@@ -2745,7 +2747,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>13</v>
       </c>
@@ -2757,7 +2759,7 @@
       <c r="E134" s="3"/>
       <c r="F134" s="2"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="3"/>
       <c r="C135" s="2"/>
@@ -2765,7 +2767,7 @@
       <c r="E135" s="3"/>
       <c r="F135" s="2"/>
     </row>
-    <row r="136" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>15</v>
       </c>
@@ -2785,7 +2787,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>8</v>
       </c>
@@ -2805,7 +2807,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>69</v>
       </c>
@@ -2825,7 +2827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>70</v>
       </c>
@@ -2845,7 +2847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>66</v>
       </c>
@@ -2865,7 +2867,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>9</v>
       </c>
@@ -2885,7 +2887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>40</v>
       </c>
@@ -2905,7 +2907,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>13</v>
       </c>
@@ -2917,7 +2919,7 @@
       <c r="E146" s="3"/>
       <c r="F146" s="2"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="3"/>
       <c r="C147" s="2"/>
@@ -2925,7 +2927,7 @@
       <c r="E147" s="3"/>
       <c r="F147" s="2"/>
     </row>
-    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>15</v>
       </c>
@@ -2945,7 +2947,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>10</v>
       </c>
@@ -2965,7 +2967,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>8</v>
       </c>
@@ -2985,19 +2987,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A154" s="4" t="s">
+    <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C154" s="2"/>
-      <c r="D154" s="3"/>
-      <c r="E154" s="3"/>
-      <c r="F154" s="2"/>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C154" s="35"/>
+      <c r="D154" s="36"/>
+      <c r="E154" s="36"/>
+      <c r="F154" s="35"/>
+      <c r="G154" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="3"/>
       <c r="C155" s="2"/>
@@ -3005,7 +3010,7 @@
       <c r="E155" s="3"/>
       <c r="F155" s="2"/>
     </row>
-    <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>15</v>
       </c>
@@ -3025,7 +3030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>10</v>
       </c>
@@ -3045,7 +3050,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="8" t="s">
         <v>8</v>
       </c>
@@ -3065,7 +3070,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
         <v>59</v>
       </c>
@@ -3085,7 +3090,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="8" t="s">
         <v>11</v>
       </c>
@@ -3105,7 +3110,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
         <v>12</v>
       </c>
@@ -3125,7 +3130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="18" t="s">
         <v>125</v>
       </c>
@@ -3146,7 +3151,7 @@
       </c>
       <c r="G162" s="21"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="10" t="s">
         <v>75</v>
       </c>
@@ -3166,7 +3171,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="9"/>
       <c r="B164" s="7"/>
       <c r="C164" s="9"/>
@@ -3174,7 +3179,7 @@
       <c r="E164" s="7"/>
       <c r="F164" s="6"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="9"/>
       <c r="B165" s="7"/>
       <c r="C165" s="9"/>
@@ -3182,7 +3187,7 @@
       <c r="E165" s="7"/>
       <c r="F165" s="6"/>
     </row>
-    <row r="167" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>13</v>
       </c>
@@ -3194,7 +3199,7 @@
       <c r="E167" s="3"/>
       <c r="F167" s="2"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="3"/>
       <c r="C168" s="2"/>
@@ -3202,7 +3207,7 @@
       <c r="E168" s="3"/>
       <c r="F168" s="2"/>
     </row>
-    <row r="169" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>15</v>
       </c>
@@ -3222,8 +3227,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A170" s="2" t="s">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="32" t="s">
         <v>76</v>
       </c>
       <c r="B170" s="3" t="s">
@@ -3241,8 +3246,11 @@
       <c r="F170" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G170" s="16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>10</v>
       </c>
@@ -3262,7 +3270,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>59</v>
       </c>
@@ -3282,7 +3290,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="18" t="s">
         <v>126</v>
       </c>
@@ -3303,7 +3311,7 @@
       </c>
       <c r="G173" s="21"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
         <v>80</v>
       </c>
@@ -3323,7 +3331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>13</v>
       </c>
@@ -3335,7 +3343,7 @@
       <c r="E178" s="3"/>
       <c r="F178" s="2"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="3"/>
       <c r="C179" s="2"/>
@@ -3343,7 +3351,7 @@
       <c r="E179" s="3"/>
       <c r="F179" s="2"/>
     </row>
-    <row r="180" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>15</v>
       </c>
@@ -3363,7 +3371,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>76</v>
       </c>
@@ -3383,7 +3391,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>10</v>
       </c>
@@ -3403,7 +3411,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>59</v>
       </c>
@@ -3423,7 +3431,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="18" t="s">
         <v>60</v>
       </c>
@@ -3444,7 +3452,7 @@
       </c>
       <c r="G184" s="21"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="18" t="s">
         <v>126</v>
       </c>
@@ -3467,7 +3475,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="18" t="s">
         <v>77</v>
       </c>
@@ -3490,7 +3498,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>13</v>
       </c>
@@ -3502,7 +3510,7 @@
       <c r="E190" s="3"/>
       <c r="F190" s="2"/>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="3"/>
       <c r="C191" s="2"/>
@@ -3510,7 +3518,7 @@
       <c r="E191" s="3"/>
       <c r="F191" s="2"/>
     </row>
-    <row r="192" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
         <v>15</v>
       </c>
@@ -3530,7 +3538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>10</v>
       </c>
@@ -3550,7 +3558,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>59</v>
       </c>
@@ -3570,7 +3578,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>82</v>
       </c>
@@ -3590,7 +3598,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="10" t="s">
         <v>83</v>
       </c>
@@ -3610,7 +3618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>84</v>
       </c>
@@ -3630,7 +3638,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
         <v>85</v>
       </c>
@@ -3650,7 +3658,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>86</v>
       </c>
@@ -3670,7 +3678,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="10" t="s">
         <v>87</v>
       </c>
@@ -3690,7 +3698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>88</v>
       </c>
@@ -3710,7 +3718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="10" t="s">
         <v>89</v>
       </c>
@@ -3730,7 +3738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>90</v>
       </c>
@@ -3750,7 +3758,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="10" t="s">
         <v>91</v>
       </c>
@@ -3770,7 +3778,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>13</v>
       </c>
@@ -3782,7 +3790,7 @@
       <c r="E208" s="3"/>
       <c r="F208" s="2"/>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="3"/>
       <c r="C209" s="2"/>
@@ -3790,7 +3798,7 @@
       <c r="E209" s="3"/>
       <c r="F209" s="2"/>
     </row>
-    <row r="210" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>15</v>
       </c>
@@ -3810,7 +3818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>93</v>
       </c>
@@ -3830,7 +3838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>95</v>
       </c>
@@ -3853,7 +3861,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
         <v>13</v>
       </c>
@@ -3865,7 +3873,7 @@
       <c r="E216" s="3"/>
       <c r="F216" s="2"/>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="3"/>
       <c r="C217" s="2"/>
@@ -3873,7 +3881,7 @@
       <c r="E217" s="3"/>
       <c r="F217" s="2"/>
     </row>
-    <row r="218" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
         <v>15</v>
       </c>
@@ -3893,7 +3901,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>93</v>
       </c>
@@ -3913,7 +3921,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>94</v>
       </c>
@@ -3931,7 +3939,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>97</v>
       </c>
@@ -3949,7 +3957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="10" t="s">
         <v>98</v>
       </c>
@@ -3967,7 +3975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="23" t="s">
         <v>99</v>
       </c>
@@ -3977,7 +3985,7 @@
       <c r="E225" s="24"/>
       <c r="F225" s="25"/>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="26"/>
       <c r="B226" s="27"/>
       <c r="C226" s="27"/>
@@ -3985,7 +3993,7 @@
       <c r="E226" s="27"/>
       <c r="F226" s="28"/>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="26"/>
       <c r="B227" s="27"/>
       <c r="C227" s="27"/>
@@ -3993,7 +4001,7 @@
       <c r="E227" s="27"/>
       <c r="F227" s="28"/>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="26"/>
       <c r="B228" s="27"/>
       <c r="C228" s="27"/>
@@ -4001,7 +4009,7 @@
       <c r="E228" s="27"/>
       <c r="F228" s="28"/>
     </row>
-    <row r="229" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="29"/>
       <c r="B229" s="30"/>
       <c r="C229" s="30"/>
@@ -4009,7 +4017,7 @@
       <c r="E229" s="30"/>
       <c r="F229" s="31"/>
     </row>
-    <row r="326" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="326" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B326" s="1">
         <v>1</v>
       </c>
@@ -4029,7 +4037,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added views for submit feedback
</commit_message>
<xml_diff>
--- a/FeedbackDatabaseDesign.xlsx
+++ b/FeedbackDatabaseDesign.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Feedback\feedback\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\myprojects\Feedback\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="131">
   <si>
     <t>effective_from</t>
   </si>
@@ -407,6 +407,12 @@
   </si>
   <si>
     <t>This is the only primary key, what is its significance?</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>What about feedback questions for lab subjects? Comments or ques?</t>
   </si>
 </sst>
 </file>
@@ -603,7 +609,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -651,6 +657,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -678,14 +693,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -995,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="G170" sqref="G170"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="C238" sqref="C238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,16 +3006,16 @@
       </c>
     </row>
     <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A154" s="33" t="s">
+      <c r="A154" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B154" s="34" t="s">
+      <c r="B154" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C154" s="35"/>
-      <c r="D154" s="36"/>
-      <c r="E154" s="36"/>
-      <c r="F154" s="35"/>
+      <c r="C154" s="26"/>
+      <c r="D154" s="27"/>
+      <c r="E154" s="27"/>
+      <c r="F154" s="26"/>
       <c r="G154" t="s">
         <v>127</v>
       </c>
@@ -3228,7 +3246,7 @@
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A170" s="32" t="s">
+      <c r="A170" s="23" t="s">
         <v>76</v>
       </c>
       <c r="B170" s="3" t="s">
@@ -3976,46 +3994,64 @@
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A225" s="23" t="s">
+      <c r="A225" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B225" s="24"/>
-      <c r="C225" s="24"/>
-      <c r="D225" s="24"/>
-      <c r="E225" s="24"/>
-      <c r="F225" s="25"/>
+      <c r="B225" s="29"/>
+      <c r="C225" s="29"/>
+      <c r="D225" s="29"/>
+      <c r="E225" s="29"/>
+      <c r="F225" s="30"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" s="26"/>
-      <c r="B226" s="27"/>
-      <c r="C226" s="27"/>
-      <c r="D226" s="27"/>
-      <c r="E226" s="27"/>
-      <c r="F226" s="28"/>
+      <c r="A226" s="31"/>
+      <c r="B226" s="32"/>
+      <c r="C226" s="32"/>
+      <c r="D226" s="32"/>
+      <c r="E226" s="32"/>
+      <c r="F226" s="33"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" s="26"/>
-      <c r="B227" s="27"/>
-      <c r="C227" s="27"/>
-      <c r="D227" s="27"/>
-      <c r="E227" s="27"/>
-      <c r="F227" s="28"/>
+      <c r="A227" s="31"/>
+      <c r="B227" s="32"/>
+      <c r="C227" s="32"/>
+      <c r="D227" s="32"/>
+      <c r="E227" s="32"/>
+      <c r="F227" s="33"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A228" s="26"/>
-      <c r="B228" s="27"/>
-      <c r="C228" s="27"/>
-      <c r="D228" s="27"/>
-      <c r="E228" s="27"/>
-      <c r="F228" s="28"/>
+      <c r="A228" s="31"/>
+      <c r="B228" s="32"/>
+      <c r="C228" s="32"/>
+      <c r="D228" s="32"/>
+      <c r="E228" s="32"/>
+      <c r="F228" s="33"/>
     </row>
     <row r="229" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="29"/>
-      <c r="B229" s="30"/>
-      <c r="C229" s="30"/>
-      <c r="D229" s="30"/>
-      <c r="E229" s="30"/>
-      <c r="F229" s="31"/>
+      <c r="A229" s="34"/>
+      <c r="B229" s="35"/>
+      <c r="C229" s="35"/>
+      <c r="D229" s="35"/>
+      <c r="E229" s="35"/>
+      <c r="F229" s="36"/>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="B234" s="38"/>
+      <c r="C234" s="37"/>
+      <c r="D234" s="38"/>
+      <c r="E234" s="38"/>
+      <c r="F234" s="37"/>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B235" s="39"/>
+      <c r="C235" s="39"/>
+      <c r="D235" s="39"/>
     </row>
     <row r="326" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B326" s="1">
@@ -4023,8 +4059,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A225:F229"/>
+    <mergeCell ref="A235:D235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>